<commit_message>
finishing coordinates proj for meanwhile
</commit_message>
<xml_diff>
--- a/GardensReader/export.xlsx
+++ b/GardensReader/export.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tzafi\Code\DogsGardenApi\GardensReader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tzafi\Code\DogsGardenApi\GardensXlsxToJson\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930"/>
   </bookViews>
   <sheets>
     <sheet name="Dog Parks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="258">
   <si>
     <t>oid_gina</t>
   </si>
@@ -108,7 +108,691 @@
     <t>חורשת ליסין</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>שטיינמן</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>חורשת שטיינמן</t>
+  </si>
+  <si>
+    <t>שכונת בבלי</t>
+  </si>
+  <si>
+    <t>7:00-22:00</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>סוטין</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>חורשת נהרדעא</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>רומנו</t>
+  </si>
+  <si>
+    <t>חורשת רומנו</t>
+  </si>
+  <si>
+    <t>פינת שחרור כלבים</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>קוסובסקי</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>גינת ראש ציפור</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>ברנדיס</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>גינת בני דן</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>יחזקאל</t>
+  </si>
+  <si>
+    <t>גן גימפל</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>ברנט</t>
+  </si>
+  <si>
+    <t>ברנט 2 פ. המרד</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>אלברט קיוסו</t>
+  </si>
+  <si>
+    <t>חורשה אלברט קיוסו</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>מעפילי אגוז</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מעפילי אגוז 73 </t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>גולי אריתריאה</t>
+  </si>
+  <si>
+    <t>הגולן 3</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>דרזנר</t>
+  </si>
+  <si>
+    <t>דרזנר מערב</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>טבריה</t>
+  </si>
+  <si>
+    <t>טבריה 1</t>
+  </si>
+  <si>
+    <t>הפרסה</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>פארק מודעי</t>
+  </si>
+  <si>
+    <t>אדירים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גן אדירים </t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>משה דיין</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>חורשת הורודצקי פ. משה דיין</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>כרם התימנים</t>
+  </si>
+  <si>
+    <t>גן הכובשים</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>רדינג 32</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>חורשת רדינג</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רמות נפתלי </t>
+  </si>
+  <si>
+    <t>גן שושני הגדול</t>
+  </si>
+  <si>
+    <t>קהילת ורשה</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>חורשת פרנקפורט</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>עופר כהן</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פארק החורשות- עופר כהן </t>
+  </si>
+  <si>
+    <t>ככר המדינה מול עקיבא אריה</t>
+  </si>
+  <si>
+    <t>בני  אפרים פ.שטרית בחורשה</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>אורי צבי גרינברג</t>
+  </si>
+  <si>
+    <t>חורשה מערבית לגן המייסדים</t>
+  </si>
+  <si>
+    <t>אשכנזי</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גן אשכנזי </t>
+  </si>
+  <si>
+    <t>רפידים</t>
+  </si>
+  <si>
+    <t>חורשת רפידים</t>
+  </si>
+  <si>
+    <t>וילנסקי</t>
+  </si>
+  <si>
+    <t>משה וילנסקי16 פ.קיפניס</t>
+  </si>
+  <si>
+    <t>מבצע קדש</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קהילת ריגא פ.מבצע קדש </t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רינגלבלום </t>
+  </si>
+  <si>
+    <t xml:space="preserve">פארק אופטושו </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ההשכלה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">שד' ההשכלה 18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">אבן גבירול בגדה הצפונית </t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>בילטמור</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גן בילטמור </t>
+  </si>
+  <si>
+    <t xml:space="preserve">השלום </t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פארק וולפסון </t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>חורשה ברחוב לאה פינת גליקסברג</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>הירקון</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>גן העצמאות מול רחוב הירקון 228</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">יהודה הלוי </t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גן קרית ספר </t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>וולפסון</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>חניון שוק גבעת עליה</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">שפע טל </t>
+  </si>
+  <si>
+    <t>רחוב שפע טל 2</t>
+  </si>
+  <si>
+    <t>לבנדה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לבנדה37 </t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>תדהר</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חורשת בני יהודה </t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ארבר מנחם </t>
+  </si>
+  <si>
+    <t>ארבר מנחם 14</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>הכובשים</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>הכובשים 78</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פארק צמרת </t>
+  </si>
+  <si>
+    <t>פינה לשחרור כלבים</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>התיבונים</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>לה גוארדיה</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לה גוארדיה 59 </t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>דובנוב</t>
+  </si>
+  <si>
+    <t>גן דובנוב</t>
+  </si>
+  <si>
+    <t>הרב אשי</t>
+  </si>
+  <si>
+    <t>גן פוליטי</t>
+  </si>
+  <si>
+    <t>וילנסקי משה</t>
+  </si>
+  <si>
+    <t>חורשת וילנסקי משה</t>
+  </si>
+  <si>
+    <t>קהילת קייב</t>
+  </si>
+  <si>
+    <t>גן אשכנזי</t>
+  </si>
+  <si>
+    <t>גן אדירים</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>גן העיר</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>מנחם מדמון</t>
+  </si>
+  <si>
+    <t>גן ראש הכפר</t>
+  </si>
+  <si>
+    <t>יגאל אלון</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>יגאל אלון 165 פינת ערבי נחל</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>תשרי</t>
+  </si>
+  <si>
+    <t>גן דגלאס</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>שגאל מרק</t>
+  </si>
+  <si>
+    <t>מרק שגאל</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>פיקוס</t>
+  </si>
+  <si>
+    <t>פיקוס 28</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>בנטוב מרדכי</t>
+  </si>
+  <si>
+    <t>בית הבילויים</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>רבנו ירוחם</t>
+  </si>
+  <si>
+    <t>חורשת רבנו ירוחם</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>מייזל זלמן</t>
+  </si>
+  <si>
+    <t>גן מייזל זלמן</t>
+  </si>
+  <si>
+    <t>דה מודינה אריה</t>
+  </si>
+  <si>
+    <t>גן דה מודינה</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>אבוקה</t>
+  </si>
+  <si>
+    <t>חורשת אבוקה 5</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>מאיר מרדכי</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>אוסישקין</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>פארק הירקון</t>
+  </si>
+  <si>
+    <t>משמר הגבול</t>
+  </si>
+  <si>
+    <t>קרן קיימת - משמר הגבול</t>
+  </si>
+  <si>
+    <t>קוממיות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קוממיות </t>
+  </si>
+  <si>
+    <t>אבן גבירול</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">אבן גבירול 213 ( בית הלוויות ) </t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>תל ברוך</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רפידים-צפון  </t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>לוינסקי</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>גן הקווקזים</t>
+  </si>
+  <si>
+    <t>פינת כלבים</t>
+  </si>
+  <si>
+    <t>טאגור</t>
+  </si>
+  <si>
+    <t>מאחורי בית השחמט</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>בויאר אברהם</t>
+  </si>
+  <si>
+    <t>חורשת בויאר אברהם</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>דניאל מוריץ</t>
+  </si>
+  <si>
+    <t>מוריץ דניאל</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">אירוס </t>
+  </si>
+  <si>
+    <t>פינת כושר</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>קהילת לודג'</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>ברלין אליהו</t>
+  </si>
+  <si>
+    <t>לאה גולדברג</t>
+  </si>
+  <si>
     <t>פארק רבין - פינת ליטוף</t>
+  </si>
+  <si>
+    <t>עקיבא אריה</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> צומת בני דן אוסישקין</t>
+  </si>
+  <si>
+    <t>צומת שטרית בני אפריים</t>
+  </si>
+  <si>
+    <t>קריאל גרדוש</t>
+  </si>
+  <si>
+    <t>שדרות בן גוריון</t>
   </si>
 </sst>
 </file>
@@ -463,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD113"/>
+      <selection activeCell="C21" sqref="C21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -526,7 +1210,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>252</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -579,6 +1263,1586 @@
       </c>
       <c r="F5" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>121</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>148</v>
+      </c>
+      <c r="F43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>161</v>
+      </c>
+      <c r="F47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>156</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>160</v>
+      </c>
+      <c r="B50" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>171</v>
+      </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" t="s">
+        <v>173</v>
+      </c>
+      <c r="F51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" t="s">
+        <v>44</v>
+      </c>
+      <c r="G52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" t="s">
+        <v>174</v>
+      </c>
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" t="s">
+        <v>175</v>
+      </c>
+      <c r="F53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>176</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>176</v>
+      </c>
+      <c r="F54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" t="s">
+        <v>177</v>
+      </c>
+      <c r="F55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>178</v>
+      </c>
+      <c r="F56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" t="s">
+        <v>81</v>
+      </c>
+      <c r="F57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" t="s">
+        <v>182</v>
+      </c>
+      <c r="F59" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" t="s">
+        <v>184</v>
+      </c>
+      <c r="E60" t="s">
+        <v>85</v>
+      </c>
+      <c r="F60" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" t="s">
+        <v>187</v>
+      </c>
+      <c r="F61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" t="s">
+        <v>188</v>
+      </c>
+      <c r="D62" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" t="s">
+        <v>190</v>
+      </c>
+      <c r="F62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>193</v>
+      </c>
+      <c r="F63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" t="s">
+        <v>196</v>
+      </c>
+      <c r="F64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" t="s">
+        <v>199</v>
+      </c>
+      <c r="F65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" t="s">
+        <v>201</v>
+      </c>
+      <c r="D66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" t="s">
+        <v>202</v>
+      </c>
+      <c r="F66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" t="s">
+        <v>204</v>
+      </c>
+      <c r="D67" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" t="s">
+        <v>205</v>
+      </c>
+      <c r="F67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>208</v>
+      </c>
+      <c r="F68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E69" t="s">
+        <v>210</v>
+      </c>
+      <c r="F69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>211</v>
+      </c>
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" t="s">
+        <v>212</v>
+      </c>
+      <c r="D70" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" t="s">
+        <v>213</v>
+      </c>
+      <c r="F70" t="s">
+        <v>44</v>
+      </c>
+      <c r="G70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" t="s">
+        <v>215</v>
+      </c>
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" t="s">
+        <v>215</v>
+      </c>
+      <c r="F71" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>216</v>
+      </c>
+      <c r="B72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D72" t="s">
+        <v>218</v>
+      </c>
+      <c r="E72" t="s">
+        <v>219</v>
+      </c>
+      <c r="F72" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" t="s">
+        <v>220</v>
+      </c>
+      <c r="D73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" t="s">
+        <v>221</v>
+      </c>
+      <c r="F73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" t="s">
+        <v>222</v>
+      </c>
+      <c r="D74" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" t="s">
+        <v>223</v>
+      </c>
+      <c r="F74" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" t="s">
+        <v>224</v>
+      </c>
+      <c r="D75" t="s">
+        <v>225</v>
+      </c>
+      <c r="E75" t="s">
+        <v>226</v>
+      </c>
+      <c r="F75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>227</v>
+      </c>
+      <c r="B76" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" t="s">
+        <v>228</v>
+      </c>
+      <c r="D76" t="s">
+        <v>65</v>
+      </c>
+      <c r="E76" t="s">
+        <v>229</v>
+      </c>
+      <c r="F76" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>230</v>
+      </c>
+      <c r="B77" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" t="s">
+        <v>231</v>
+      </c>
+      <c r="D77" t="s">
+        <v>232</v>
+      </c>
+      <c r="E77" t="s">
+        <v>233</v>
+      </c>
+      <c r="F77" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>158</v>
+      </c>
+      <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" t="s">
+        <v>235</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" t="s">
+        <v>236</v>
+      </c>
+      <c r="F78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>237</v>
+      </c>
+      <c r="B79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" t="s">
+        <v>238</v>
+      </c>
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" t="s">
+        <v>239</v>
+      </c>
+      <c r="F79" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>240</v>
+      </c>
+      <c r="C80" t="s">
+        <v>241</v>
+      </c>
+      <c r="D80" t="s">
+        <v>93</v>
+      </c>
+      <c r="E80" t="s">
+        <v>242</v>
+      </c>
+      <c r="F80" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>243</v>
+      </c>
+      <c r="C81" t="s">
+        <v>241</v>
+      </c>
+      <c r="D81" t="s">
+        <v>93</v>
+      </c>
+      <c r="E81" t="s">
+        <v>242</v>
+      </c>
+      <c r="F81" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" t="s">
+        <v>244</v>
+      </c>
+      <c r="D82" t="s">
+        <v>80</v>
+      </c>
+      <c r="E82" t="s">
+        <v>202</v>
+      </c>
+      <c r="F82" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>246</v>
+      </c>
+      <c r="B83" t="s">
+        <v>247</v>
+      </c>
+      <c r="C83" t="s">
+        <v>248</v>
+      </c>
+      <c r="D83" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>249</v>
+      </c>
+      <c r="C84" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" t="s">
+        <v>250</v>
+      </c>
+      <c r="F84" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>